<commit_message>
Added test for password toggle
</commit_message>
<xml_diff>
--- a/src/test/resources/DataProviderFiles/negative-cases-for-login.xlsx
+++ b/src/test/resources/DataProviderFiles/negative-cases-for-login.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -129,13 +129,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -159,103 +163,83 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="229.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="100.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="12.64"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" display="aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa@example.com"/>
     <hyperlink ref="A6" r:id="rId2" display="alice@mail.com"/>
     <hyperlink ref="A7" r:id="rId3" display="alice@mail.com"/>
-    <hyperlink ref="A8" r:id="rId4" display="alice@mail.com"/>
-    <hyperlink ref="A9" r:id="rId5" display="alice@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>